<commit_message>
added partially 22 gas
</commit_message>
<xml_diff>
--- a/reporte_estadistico/data/gas/metricsCategorias/metrics_21/cat3/metrics_data_vcon.xlsx
+++ b/reporte_estadistico/data/gas/metricsCategorias/metrics_21/cat3/metrics_data_vcon.xlsx
@@ -1,21 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\JJ\repos\research_eslatina\reporte_estadistico\data\gas\metricsCategorias\metrics_21\cat3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="236" yWindow="13" windowWidth="16089" windowHeight="9661"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>quant0</t>
+  </si>
+  <si>
+    <t>quant25</t>
+  </si>
+  <si>
+    <t>quant50</t>
+  </si>
+  <si>
+    <t>quant75</t>
+  </si>
+  <si>
+    <t>quant100</t>
+  </si>
+  <si>
+    <t>skewness</t>
+  </si>
+  <si>
+    <t>kurtosis</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>std_dev</t>
+  </si>
+  <si>
+    <t>variance</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>Estrato1_vcon</t>
+  </si>
+  <si>
+    <t>Estrato2_vcon</t>
+  </si>
+  <si>
+    <t>Estrato3_vcon</t>
+  </si>
+  <si>
+    <t>Estrato4_vcon</t>
+  </si>
+  <si>
+    <t>Estrato5_vcon</t>
+  </si>
+  <si>
+    <t>Estrato6_vcon</t>
+  </si>
+  <si>
+    <t>totResidencial_vcon</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,11 +130,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -109,7 +184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +216,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +251,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,120 +427,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>quant0</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>quant25</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>quant50</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>quant75</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>quant100</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>skewness</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>kurtosis</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>median</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>std_dev</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>variance</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>mean</t>
-        </is>
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Estrato1_vcon</t>
-        </is>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>0.419171</v>
+        <v>0.41917100000000002</v>
       </c>
       <c r="C2">
         <v>123.44136405</v>
       </c>
       <c r="D2">
-        <v>303.140134</v>
+        <v>303.14013399999999</v>
       </c>
       <c r="E2">
-        <v>494.670709</v>
+        <v>494.67070899999999</v>
       </c>
       <c r="F2">
-        <v>821.892864</v>
+        <v>821.89286400000003</v>
       </c>
       <c r="G2">
-        <v>0.2709254744829602</v>
+        <v>0.27092547448296023</v>
       </c>
       <c r="H2">
         <v>1.771360127566971</v>
       </c>
       <c r="I2">
-        <v>303.140134</v>
+        <v>303.14013399999999</v>
       </c>
       <c r="J2">
         <v>215.529776399632</v>
       </c>
       <c r="K2">
-        <v>46453.08451487537</v>
+        <v>46453.084514875372</v>
       </c>
       <c r="L2">
-        <v>313.8678031990729</v>
+        <v>313.86780319907291</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Estrato2_vcon</t>
-        </is>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -472,22 +521,22 @@
         <v>201.9594352</v>
       </c>
       <c r="D3">
-        <v>317.90811495</v>
+        <v>317.90811495000003</v>
       </c>
       <c r="E3">
-        <v>420.328590805</v>
+        <v>420.32859080499998</v>
       </c>
       <c r="F3">
-        <v>783.18494673</v>
+        <v>783.18494672999998</v>
       </c>
       <c r="G3">
-        <v>0.2691579033373572</v>
+        <v>0.26915790333735717</v>
       </c>
       <c r="H3">
-        <v>2.427579808534957</v>
+        <v>2.4275798085349569</v>
       </c>
       <c r="I3">
-        <v>317.90811495</v>
+        <v>317.90811495000003</v>
       </c>
       <c r="J3">
         <v>177.485750983966</v>
@@ -496,14 +545,12 @@
         <v>31501.1918023424</v>
       </c>
       <c r="L3">
-        <v>324.075799975894</v>
+        <v>324.07579997589397</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Estrato3_vcon</t>
-        </is>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -515,35 +562,33 @@
         <v>15.910295</v>
       </c>
       <c r="E4">
-        <v>85.40487044</v>
+        <v>85.404870439999996</v>
       </c>
       <c r="F4">
-        <v>334.30374443</v>
+        <v>334.30374442999999</v>
       </c>
       <c r="G4">
         <v>1.367273799593842</v>
       </c>
       <c r="H4">
-        <v>3.767967101830138</v>
+        <v>3.7679671018301382</v>
       </c>
       <c r="I4">
         <v>15.910295</v>
       </c>
       <c r="J4">
-        <v>79.4804301980038</v>
+        <v>79.480430198003802</v>
       </c>
       <c r="K4">
-        <v>6317.138784459755</v>
+        <v>6317.1387844597548</v>
       </c>
       <c r="L4">
-        <v>58.85284565165563</v>
+        <v>58.852845651655628</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Estrato4_vcon</t>
-        </is>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -555,16 +600,16 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1.2045985</v>
+        <v>1.2045984999999999</v>
       </c>
       <c r="F5">
         <v>115.301671</v>
       </c>
       <c r="G5">
-        <v>4.086613347768203</v>
+        <v>4.0866133477682034</v>
       </c>
       <c r="H5">
-        <v>21.41063658879212</v>
+        <v>21.410636588792119</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -573,17 +618,15 @@
         <v>20.38692394195504</v>
       </c>
       <c r="K5">
-        <v>415.6266678150598</v>
+        <v>415.62666781505982</v>
       </c>
       <c r="L5">
         <v>6.057339843311258</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Estrato5_vcon</t>
-        </is>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -598,26 +641,24 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>79.233479</v>
+        <v>79.233479000000003</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>6.560121316982468</v>
+        <v>6.5601213169824684</v>
       </c>
       <c r="K6">
-        <v>43.03519169352779</v>
+        <v>43.035191693527793</v>
       </c>
       <c r="L6">
-        <v>0.7139464357615895</v>
+        <v>0.71394643576158945</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Estrato6_vcon</t>
-        </is>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -632,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>7.438263</v>
+        <v>7.4382630000000001</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -641,35 +682,33 @@
         <v>0.6236933480612562</v>
       </c>
       <c r="K7">
-        <v>0.3889933924158592</v>
+        <v>0.38899339241585917</v>
       </c>
       <c r="L7">
-        <v>0.06803178721854304</v>
+        <v>6.8031787218543041E-2</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>totResidencial_vcon</t>
-        </is>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
       </c>
       <c r="B8">
-        <v>258.795994</v>
+        <v>258.79599400000001</v>
       </c>
       <c r="C8">
-        <v>530.4406143900001</v>
+        <v>530.44061439000006</v>
       </c>
       <c r="D8">
         <v>677.511799</v>
       </c>
       <c r="E8">
-        <v>851.043286555</v>
+        <v>851.04328655500001</v>
       </c>
       <c r="F8">
         <v>1476.31077</v>
       </c>
       <c r="G8">
-        <v>0.01733882277532653</v>
+        <v>1.7338822775326529E-2</v>
       </c>
       <c r="H8">
         <v>1.900957422951369</v>
@@ -678,13 +717,13 @@
         <v>677.511799</v>
       </c>
       <c r="J8">
-        <v>223.8791924718734</v>
+        <v>223.87919247187341</v>
       </c>
       <c r="K8">
         <v>50121.89282185815</v>
       </c>
       <c r="L8">
-        <v>703.6357668929139</v>
+        <v>703.63576689291392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>